<commit_message>
fixed: a problem causing prices not to update in exported .ekap file
</commit_message>
<xml_diff>
--- a/dev/veri/dsi/output.xlsx
+++ b/dev/veri/dsi/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\ekap-editor\dev\veri\dsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8F2864-3837-4A01-B58F-A9A52CC59AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87EB899-FEE1-46A9-AF05-AF84C1B1E026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17744,48 +17744,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="162"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="162"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -17980,6 +17938,48 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
         <color auto="1"/>
         <name val="Calibri"/>
         <family val="2"/>
@@ -18085,16 +18085,16 @@
     <tableColumn id="2" xr3:uid="{B1665020-F315-41C6-8908-96B02BD44363}" name="DESCRIPTION" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{B86E0FCC-97A4-4EE3-BBAE-0EAE1E43AE70}" name="UNIT" dataDxfId="11"/>
     <tableColumn id="4" xr3:uid="{EF48DF9F-740B-4709-A520-94E33131919F}" name="UNIT_PRICE" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{A603D460-C3A7-4149-B0E3-81FAE63A8ADB}" name="MONTAGE_PRICE" dataDxfId="0"/>
-    <tableColumn id="13" xr3:uid="{0C7659E3-3E31-42C8-80C6-BFD36F8B1723}" name="DEMONTAGE_PRICE" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{48A09BB2-93E5-4EF0-849D-AA6E1B97EF68}" name="DESCRIPTION_PREFIX" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{EFB94B16-573E-4C22-B993-698AF2478455}" name="DESCRIPTION_SUFFIX" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{79B1E16D-57BD-40F9-B4F8-E2438F8B702B}" name="CATEGORY" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{15DB3D6E-AC89-4BFC-9EAA-8A635183C875}" name="SUB_CATEGORY" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{43A2A40C-5EAC-446F-9A75-8C89DFE721B8}" name="BOOK" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{247CA465-91C2-43A5-9847-E3CAD2C1EA8B}" name="BOOK_YEAR" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{1B1DD5E6-68E0-482C-87B3-15A186661440}" name="BOOK_MONTH" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{ACED9485-8D7B-4B20-9DB0-8238BEA57E72}" name="BOOK_LINK" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{A603D460-C3A7-4149-B0E3-81FAE63A8ADB}" name="MONTAGE_PRICE" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{0C7659E3-3E31-42C8-80C6-BFD36F8B1723}" name="DEMONTAGE_PRICE" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{48A09BB2-93E5-4EF0-849D-AA6E1B97EF68}" name="DESCRIPTION_PREFIX" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{EFB94B16-573E-4C22-B993-698AF2478455}" name="DESCRIPTION_SUFFIX" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{79B1E16D-57BD-40F9-B4F8-E2438F8B702B}" name="CATEGORY" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{15DB3D6E-AC89-4BFC-9EAA-8A635183C875}" name="SUB_CATEGORY" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{43A2A40C-5EAC-446F-9A75-8C89DFE721B8}" name="BOOK" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{247CA465-91C2-43A5-9847-E3CAD2C1EA8B}" name="BOOK_YEAR" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{1B1DD5E6-68E0-482C-87B3-15A186661440}" name="BOOK_MONTH" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{ACED9485-8D7B-4B20-9DB0-8238BEA57E72}" name="BOOK_LINK" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -18423,8 +18423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N1979"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="H111" sqref="H111"/>
+    <sheetView tabSelected="1" topLeftCell="A1948" workbookViewId="0">
+      <selection activeCell="E1986" sqref="E1986"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>

</xml_diff>